<commit_message>
updated the R code
</commit_message>
<xml_diff>
--- a/R/Hanqing_Liu_CGM_SpeakerInfoRequest.xlsx
+++ b/R/Hanqing_Liu_CGM_SpeakerInfoRequest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanqing/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jyang21/Documents/website/cgmonline/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAF761F-3F5E-7A41-A0D6-189618241D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6060E8DD-0E47-6042-8C7F-7F43152C3EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="500" windowWidth="29620" windowHeight="18700" xr2:uid="{3C3BDFD3-7B9B-4756-8DF6-B516485A172E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>[演讲题目]</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>Mammalian brain cells show remarkable diversity in gene expression, anatomy and function, yet the regulatory DNA landscape underlying this extensive heterogeneity is poorly understood. Here we carry out a comprehensive assessment of the epigenomes of mouse brain cell types by applying single-nucleus DNA methylation sequencing1,2 to profile 103,982 nuclei (including 95,815 neurons and 8,167 non-neuronal cells) from 45 regions of the mouse cortex, hippocampus, striatum, pallidum and olfactory areas. We identified 161 cell clusters with distinct spatial locations and projection targets. We constructed taxonomies of these epigenetic types, annotated with signature genes, regulatory elements and transcription factors. These features indicate the potential regulatory landscape supporting the assignment of putative cell types and reveal repetitive usage of regulators in excitatory and inhibitory cells for determining subtypes. The DNA methylation landscape of excitatory neurons in the cortex and hippocampus varied continuously along spatial gradients. Using this deep dataset, we constructed an artificial neural network model that precisely predicts single neuron cell-type identity and brain area spatial location. Integration of high-resolution DNA methylomes with single-nucleus chromatin accessibility data3 enabled prediction of high-confidence enhancer–gene interactions for all identified cell types, which were subsequently validated by cell-type-specific chromatin conformation capture experiments4. By combining multi-omic datasets (DNA methylation, chromatin contacts, and open chromatin) from single nuclei and annotating the regulatory genome of hundreds of cell types in the mouse brain, our DNA methylation atlas establishes the epigenetic basis for neuronal diversity and spatial organization throughout the mouse cerebrum.</t>
+  </si>
+  <si>
+    <t>"03-30-2022"</t>
   </si>
 </sst>
 </file>
@@ -247,9 +250,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8ED7A4-1226-41E2-9D92-4601711E979C}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -593,6 +597,9 @@
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>